<commit_message>
Changed Teststep for TC22 - Prod
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC22_Verify_PDP_Page.xlsx
+++ b/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC22_Verify_PDP_Page.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranchOCT2021\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_Muitisite\Input_files\Actual_testcases\Kaman\Prod\KIT\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E361E402-5DD5-4651-AC1E-70904EE29D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F127646B-4CD7-41FB-B4E7-90F752C09B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="54">
   <si>
     <t>TestCase</t>
   </si>
@@ -68,9 +68,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>$BaseURL</t>
-  </si>
-  <si>
     <t>VERIFY_WEBELEMENT_PRESENT</t>
   </si>
   <si>
@@ -183,6 +180,9 @@
   </si>
   <si>
     <t>$86.30</t>
+  </si>
+  <si>
+    <t>$BaseURLKIT</t>
   </si>
 </sst>
 </file>
@@ -629,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +663,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>5</v>
@@ -720,7 +720,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>8</v>
@@ -742,7 +742,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>8</v>
@@ -755,7 +755,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>8</v>
@@ -768,7 +768,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>8</v>
@@ -809,37 +809,37 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="D15" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="8"/>
@@ -848,16 +848,16 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -872,217 +872,211 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="10" t="s">
-        <v>41</v>
+      <c r="B21" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="9" t="s">
-        <v>16</v>
+      <c r="B22" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="10" t="s">
-        <v>41</v>
+      <c r="B23" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="9" t="s">
-        <v>16</v>
+      <c r="B24" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="10" t="s">
-        <v>41</v>
+      <c r="B25" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="9" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="9" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="9" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
-      <c r="B33" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="B33" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="10" t="s">
-        <v>10</v>
+      <c r="B34" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="8"/>
@@ -1091,16 +1085,22 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>28</v>
@@ -1115,7 +1115,7 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>29</v>
@@ -1130,7 +1130,7 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>30</v>
@@ -1145,31 +1145,31 @@
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>37</v>
@@ -1184,7 +1184,7 @@
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>38</v>
@@ -1199,7 +1199,7 @@
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>39</v>
@@ -1209,21 +1209,6 @@
       </c>
       <c r="E43" s="6" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1235,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,12 +1243,12 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="6" t="b">
         <v>1</v>
@@ -1271,7 +1256,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="6" t="b">
         <v>1</v>
@@ -1279,7 +1264,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6" t="b">
         <v>1</v>
@@ -1287,7 +1272,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6" t="b">
         <v>1</v>
@@ -1295,15 +1280,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="b">
         <v>1</v>
@@ -1311,15 +1296,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="6" t="b">
         <v>1</v>
@@ -1327,15 +1312,15 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="6" t="b">
         <v>1</v>
@@ -1343,7 +1328,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="6" t="b">
         <v>1</v>
@@ -1351,7 +1336,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="6" t="b">
         <v>1</v>
@@ -1359,7 +1344,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="15" t="b">
         <v>1</v>
@@ -1367,7 +1352,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="6" t="b">
         <v>1</v>
@@ -1375,7 +1360,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="6">
         <v>123806</v>
@@ -1383,7 +1368,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="6" t="b">
         <v>1</v>
@@ -1391,15 +1376,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="6" t="b">
         <v>1</v>
@@ -1407,7 +1392,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="6" t="b">
         <v>1</v>
@@ -1415,7 +1400,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="6" t="b">
         <v>1</v>
@@ -1423,7 +1408,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="6" t="b">
         <v>1</v>
@@ -1431,7 +1416,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="12" t="b">
         <v>1</v>
@@ -1439,7 +1424,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="12" t="b">
         <v>1</v>
@@ -1447,7 +1432,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="6" t="b">
         <v>1</v>
@@ -1455,7 +1440,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="12" t="b">
         <v>1</v>
@@ -1463,7 +1448,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="12" t="b">
         <v>1</v>

</xml_diff>